<commit_message>
Fixed EAC, now within 1%
</commit_message>
<xml_diff>
--- a/EVA.xlsx
+++ b/EVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\source\repos\ProjMan412\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06100BC3-4CFB-4068-A89A-1C53F010AD71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC81135-6542-482A-92D8-DD42FDFD1525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3051,7 +3051,7 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3102,10 +3102,10 @@
         <v>0.93659999999999999</v>
       </c>
       <c r="H3">
-        <v>3779.6399000000001</v>
+        <v>310324.01679999998</v>
       </c>
       <c r="I3">
-        <v>59607.5599</v>
+        <v>366151.93679999997</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -3128,10 +3128,10 @@
         <v>0.80500000000000005</v>
       </c>
       <c r="H4">
-        <v>22488.918699999998</v>
+        <v>281630.15049999999</v>
       </c>
       <c r="I4">
-        <v>115301.42869999999</v>
+        <v>374442.6605</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -3153,11 +3153,11 @@
       <c r="G5">
         <v>0.89200000000000002</v>
       </c>
-      <c r="H5">
-        <v>18552.309499999999</v>
+      <c r="H5" s="1">
+        <v>221024.93049999999</v>
       </c>
       <c r="I5">
-        <v>171819.36550000001</v>
+        <v>374291.9865</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -3180,10 +3180,10 @@
         <v>0.88060000000000005</v>
       </c>
       <c r="H6">
-        <v>23499.718099999998</v>
+        <v>199315.78150000001</v>
       </c>
       <c r="I6">
-        <v>196795.46410000001</v>
+        <v>372611.52750000003</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -3206,10 +3206,10 @@
         <v>0.84719999999999995</v>
       </c>
       <c r="H7">
-        <v>35990.911399999997</v>
+        <v>170113.35829999999</v>
       </c>
       <c r="I7">
-        <v>235495.00140000001</v>
+        <v>369617.44830000005</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -3232,10 +3232,10 @@
         <v>0.87790000000000001</v>
       </c>
       <c r="H8">
-        <v>33240.022400000002</v>
+        <v>138404.2824</v>
       </c>
       <c r="I8">
-        <v>272201.05240000004</v>
+        <v>377365.31240000005</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -3258,10 +3258,10 @@
         <v>0.81210000000000004</v>
       </c>
       <c r="H9">
-        <v>62919.719400000002</v>
+        <v>112584.6713</v>
       </c>
       <c r="I9">
-        <v>334928.02940000006</v>
+        <v>384592.98130000004</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -3284,10 +3284,10 @@
         <v>0.86980000000000002</v>
       </c>
       <c r="H10">
-        <v>45512.501300000004</v>
+        <v>83388.278399999996</v>
       </c>
       <c r="I10">
-        <v>349466.16830000014</v>
+        <v>387341.94540000014</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -3310,10 +3310,10 @@
         <v>0.86860000000000004</v>
       </c>
       <c r="H11">
-        <v>48046.530899999998</v>
-      </c>
-      <c r="I11">
-        <v>365594.95950000011</v>
+        <v>68865.987999999998</v>
+      </c>
+      <c r="I11" s="1">
+        <v>386414.41660000011</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -3336,10 +3336,10 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="H12">
-        <v>33826.775699999998</v>
+        <v>46593.948799999998</v>
       </c>
       <c r="I12">
-        <v>371709.42570000014</v>
+        <v>384476.59880000015</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -6546,8 +6546,8 @@
         <v>46</v>
       </c>
       <c r="C76" s="1">
-        <f>ROUND((I71-L71)/C74,4)</f>
-        <v>48046.530899999998</v>
+        <f>ROUND((296072-L71)/C74,4)</f>
+        <v>68865.987999999998</v>
       </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
@@ -6556,7 +6556,7 @@
       </c>
       <c r="C77" s="1">
         <f>N71+C76</f>
-        <v>365594.95950000011</v>
+        <v>386414.41660000011</v>
       </c>
     </row>
   </sheetData>
@@ -10187,8 +10187,8 @@
         <v>46</v>
       </c>
       <c r="C83" s="1">
-        <f>ROUND((I78-L78)/C81,4)</f>
-        <v>33826.775699999998</v>
+        <f>ROUND((296072-L78)/C81,4)</f>
+        <v>46593.948799999998</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
@@ -10197,7 +10197,7 @@
       </c>
       <c r="C84" s="1">
         <f>N78+C83</f>
-        <v>371709.42570000014</v>
+        <v>384476.59880000015</v>
       </c>
     </row>
   </sheetData>
@@ -13818,7 +13818,7 @@
         <v>46</v>
       </c>
       <c r="C83" s="1">
-        <f>ROUND((I78-L78)/C81,4)</f>
+        <f>ROUND((296072-L78)/C81,4)</f>
         <v>17657.704900000001</v>
       </c>
     </row>
@@ -14020,8 +14020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1305C3EB-2F84-4D2C-9CBD-BEE4F9B068A0}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17412,7 +17412,10 @@
       <c r="E78" s="21"/>
       <c r="F78" s="1"/>
       <c r="G78" s="21"/>
-      <c r="H78" s="20"/>
+      <c r="H78" s="20">
+        <f>SUM(H7:H76)</f>
+        <v>296072</v>
+      </c>
       <c r="I78" s="20">
         <f>SUM(I7:I76)</f>
         <v>296072</v>
@@ -17452,7 +17455,7 @@
         <v>46</v>
       </c>
       <c r="C83" s="1">
-        <f>ROUND((I78-L78)/C81,4)</f>
+        <f>ROUND((296072-L78)/C81,4)</f>
         <v>2242.2954</v>
       </c>
     </row>
@@ -18370,8 +18373,8 @@
         <v>46</v>
       </c>
       <c r="C23" s="1">
-        <f>ROUND((I19-L19)/C21,4)</f>
-        <v>3779.6399000000001</v>
+        <f>ROUND((296072-L19)/C21,4)</f>
+        <v>310324.01679999998</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
@@ -18380,7 +18383,7 @@
       </c>
       <c r="C24" s="1">
         <f>N19+C23</f>
-        <v>59607.5599</v>
+        <v>366151.93679999997</v>
       </c>
     </row>
   </sheetData>
@@ -19475,8 +19478,8 @@
         <v>46</v>
       </c>
       <c r="C29" s="1">
-        <f>ROUND((I25-L25)/C27,4)</f>
-        <v>22488.918699999998</v>
+        <f>ROUND((296072-L25)/C27,4)</f>
+        <v>281630.15049999999</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -19485,7 +19488,7 @@
       </c>
       <c r="C30" s="1">
         <f>N25+C29</f>
-        <v>115301.42869999999</v>
+        <v>374442.6605</v>
       </c>
     </row>
   </sheetData>
@@ -20788,8 +20791,8 @@
         <v>46</v>
       </c>
       <c r="C35" s="1">
-        <f>ROUND((I31-L31)/C33,4)</f>
-        <v>18552.309499999999</v>
+        <f>ROUND((296072-L31)/C33,4)</f>
+        <v>221024.93049999999</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -20798,7 +20801,7 @@
       </c>
       <c r="C36" s="1">
         <f>N31+C35</f>
-        <v>171819.36550000001</v>
+        <v>374291.9865</v>
       </c>
     </row>
   </sheetData>
@@ -22371,8 +22374,8 @@
         <v>46</v>
       </c>
       <c r="C40" s="1">
-        <f>ROUND((I36-L36)/C38,4)</f>
-        <v>23499.718099999998</v>
+        <f>ROUND((296072-L36)/C38,4)</f>
+        <v>199315.78150000001</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
@@ -22381,7 +22384,7 @@
       </c>
       <c r="C41" s="1">
         <f>N36+C40</f>
-        <v>196795.46410000001</v>
+        <v>372611.52750000003</v>
       </c>
     </row>
   </sheetData>
@@ -22474,7 +22477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF63442B-36FE-4536-AF6A-F902A9F96283}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -24246,8 +24249,8 @@
         <v>46</v>
       </c>
       <c r="C46" s="1">
-        <f>ROUND((I42-L42)/C44,4)</f>
-        <v>35990.911399999997</v>
+        <f>ROUND((296072-L42)/C44,4)</f>
+        <v>170113.35829999999</v>
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
@@ -24256,7 +24259,7 @@
       </c>
       <c r="C47" s="1">
         <f>N42+C46</f>
-        <v>235495.00140000001</v>
+        <v>369617.44830000005</v>
       </c>
     </row>
   </sheetData>
@@ -26750,8 +26753,8 @@
         <v>46</v>
       </c>
       <c r="C58" s="1">
-        <f>ROUND((I54-L54)/C56,4)</f>
-        <v>33240.022400000002</v>
+        <f>ROUND((296072-L54)/C56,4)</f>
+        <v>138404.2824</v>
       </c>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
@@ -26760,7 +26763,7 @@
       </c>
       <c r="C59" s="1">
         <f>N54+C58</f>
-        <v>272201.05240000004</v>
+        <v>377365.31240000005</v>
       </c>
     </row>
   </sheetData>
@@ -29752,8 +29755,8 @@
         <v>46</v>
       </c>
       <c r="C70" s="1">
-        <f>ROUND((I65-L65)/C68,4)</f>
-        <v>62919.719400000002</v>
+        <f>ROUND((296072-L65)/C68,4)</f>
+        <v>112584.6713</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
@@ -29762,7 +29765,7 @@
       </c>
       <c r="C71" s="1">
         <f>N65+C70</f>
-        <v>334928.02940000006</v>
+        <v>384592.98130000004</v>
       </c>
     </row>
   </sheetData>
@@ -33100,8 +33103,8 @@
         <v>46</v>
       </c>
       <c r="C76" s="1">
-        <f>ROUND((I71-L71)/C74,4)</f>
-        <v>45512.501300000004</v>
+        <f>ROUND((296072-L71)/C74,4)</f>
+        <v>83388.278399999996</v>
       </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
@@ -33110,7 +33113,7 @@
       </c>
       <c r="C77" s="1">
         <f>N71+C76</f>
-        <v>349466.16830000014</v>
+        <v>387341.94540000014</v>
       </c>
     </row>
   </sheetData>
@@ -33339,21 +33342,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071653D7A7AD0F042B81CC9D7104BD79A" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53cf290c298691ee1eefd73e74fdead6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d6c70525-6c7a-4f52-b73c-2c8400edbf08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65d72cc0c5b6c426c55d70069f464dc3" ns2:_="">
     <xsd:import namespace="d6c70525-6c7a-4f52-b73c-2c8400edbf08"/>
@@ -33529,24 +33517,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA3C3E4-7362-49E3-85D1-432ABD3BF726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97440079-3730-432A-B1FC-864C0EBAE3CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F13AC17-8982-4195-84C9-077EA8A26B78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33562,4 +33548,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97440079-3730-432A-B1FC-864C0EBAE3CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA3C3E4-7362-49E3-85D1-432ABD3BF726}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>